<commit_message>
Add graph of age at election, focused on PMs
</commit_message>
<xml_diff>
--- a/data/misc/misc_elections_data.xlsx
+++ b/data/misc/misc_elections_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rohanalexander/Documents/phd/hansard/data/politicians/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rohanalexander/Documents/phd/hansard/data/misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38B2F01F-725C-074B-87E7-F332464A3F01}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30951456-8282-6C47-9D48-08E398B14AC9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-47320" yWindow="-9520" windowWidth="27640" windowHeight="16540" xr2:uid="{BF753662-51A7-C348-9337-8D82CA069EB9}"/>
+    <workbookView xWindow="-30820" yWindow="-10340" windowWidth="22920" windowHeight="23560" xr2:uid="{BF753662-51A7-C348-9337-8D82CA069EB9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,17 +23,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="67">
   <si>
     <t>electionDate</t>
   </si>
@@ -44,15 +39,6 @@
     <t>year</t>
   </si>
   <si>
-    <t>1901</t>
-  </si>
-  <si>
-    <t>1903</t>
-  </si>
-  <si>
-    <t>1906</t>
-  </si>
-  <si>
     <t>13 April 1910</t>
   </si>
   <si>
@@ -191,9 +177,6 @@
     <t>Lyons '31</t>
   </si>
   <si>
-    <t>Cutin '43</t>
-  </si>
-  <si>
     <t>Menzies '49</t>
   </si>
   <si>
@@ -213,6 +196,39 @@
   </si>
   <si>
     <t>comment</t>
+  </si>
+  <si>
+    <t>29 March 1901</t>
+  </si>
+  <si>
+    <t>16 December 1903</t>
+  </si>
+  <si>
+    <t>12 December 1906</t>
+  </si>
+  <si>
+    <t>Curtin '43</t>
+  </si>
+  <si>
+    <t>Hughes '19</t>
+  </si>
+  <si>
+    <t>Scullin '29</t>
+  </si>
+  <si>
+    <t>Lyons '34</t>
+  </si>
+  <si>
+    <t>Menzies '51</t>
+  </si>
+  <si>
+    <t>Menzies '55</t>
+  </si>
+  <si>
+    <t>Hawke '87</t>
+  </si>
+  <si>
+    <t>First election</t>
   </si>
 </sst>
 </file>
@@ -568,13 +584,14 @@
   <dimension ref="A1:F121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="3" max="3" width="17.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11" customWidth="1"/>
+    <col min="5" max="5" width="11" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -588,13 +605,13 @@
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F1" t="s">
-        <v>59</v>
+        <v>53</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -605,10 +622,16 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" t="s">
-        <v>48</v>
+        <v>56</v>
+      </c>
+      <c r="D2">
+        <v>75</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -624,10 +647,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" t="s">
-        <v>48</v>
+        <v>57</v>
+      </c>
+      <c r="D4">
+        <v>75</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -648,10 +674,13 @@
         <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" t="s">
-        <v>48</v>
+        <v>58</v>
+      </c>
+      <c r="D7">
+        <v>75</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -677,13 +706,13 @@
         <v>1</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D11">
         <v>75</v>
       </c>
-      <c r="E11" t="s">
-        <v>49</v>
+      <c r="E11" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -704,13 +733,13 @@
         <v>1</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D14">
         <v>75</v>
       </c>
-      <c r="E14" t="s">
-        <v>48</v>
+      <c r="E14" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -721,16 +750,16 @@
         <v>1</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D15">
         <v>75</v>
       </c>
-      <c r="E15" t="s">
-        <v>49</v>
-      </c>
-      <c r="F15" t="s">
-        <v>50</v>
+      <c r="E15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -751,13 +780,13 @@
         <v>1</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D18">
         <v>75</v>
       </c>
-      <c r="E18" t="s">
-        <v>48</v>
+      <c r="E18" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -773,13 +802,16 @@
         <v>1</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D20">
         <v>75</v>
       </c>
-      <c r="E20" t="s">
-        <v>48</v>
+      <c r="E20" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -800,13 +832,13 @@
         <v>1</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D23">
         <v>75</v>
       </c>
-      <c r="E23" t="s">
-        <v>48</v>
+      <c r="E23" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -827,13 +859,13 @@
         <v>1</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D26">
         <v>75</v>
       </c>
-      <c r="E26" t="s">
-        <v>48</v>
+      <c r="E26" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -854,13 +886,13 @@
         <v>1</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D29">
         <v>75</v>
       </c>
-      <c r="E29" t="s">
-        <v>48</v>
+      <c r="E29" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -871,13 +903,16 @@
         <v>1</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D30">
         <v>75</v>
       </c>
-      <c r="E30" t="s">
-        <v>49</v>
+      <c r="E30" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -893,16 +928,16 @@
         <v>1</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D32">
         <v>75</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E32" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F32" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="F32" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -923,13 +958,16 @@
         <v>1</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D35">
         <v>74</v>
       </c>
-      <c r="E35" t="s">
-        <v>48</v>
+      <c r="E35" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -950,13 +988,13 @@
         <v>1</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D38">
         <v>74</v>
       </c>
-      <c r="E38" t="s">
-        <v>48</v>
+      <c r="E38" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -977,13 +1015,13 @@
         <v>1</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D41">
         <v>74</v>
       </c>
-      <c r="E41" t="s">
-        <v>48</v>
+      <c r="E41" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -1004,16 +1042,16 @@
         <v>1</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D44">
         <v>74</v>
       </c>
-      <c r="E44" t="s">
-        <v>49</v>
-      </c>
-      <c r="F44" t="s">
-        <v>52</v>
+      <c r="E44" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -1034,13 +1072,13 @@
         <v>1</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D47">
         <v>74</v>
       </c>
-      <c r="E47" t="s">
-        <v>49</v>
+      <c r="E47" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -1061,16 +1099,16 @@
         <v>1</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D50">
         <v>121</v>
       </c>
-      <c r="E50" t="s">
-        <v>48</v>
-      </c>
-      <c r="F50" t="s">
-        <v>53</v>
+      <c r="E50" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -1086,13 +1124,16 @@
         <v>1</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D52">
         <v>121</v>
       </c>
-      <c r="E52" t="s">
-        <v>48</v>
+      <c r="E52" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -1113,13 +1154,13 @@
         <v>1</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D55">
         <v>121</v>
       </c>
-      <c r="E55" t="s">
-        <v>48</v>
+      <c r="E55" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -1130,13 +1171,16 @@
         <v>1</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D56">
         <v>122</v>
       </c>
-      <c r="E56" t="s">
-        <v>48</v>
+      <c r="E56" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -1157,13 +1201,13 @@
         <v>1</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D59">
         <v>122</v>
       </c>
-      <c r="E59" t="s">
-        <v>48</v>
+      <c r="E59" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -1184,13 +1228,13 @@
         <v>1</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D62">
         <v>122</v>
       </c>
-      <c r="E62" t="s">
-        <v>48</v>
+      <c r="E62" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -1206,13 +1250,13 @@
         <v>1</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D64">
         <v>122</v>
       </c>
-      <c r="E64" t="s">
-        <v>48</v>
+      <c r="E64" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -1233,13 +1277,13 @@
         <v>1</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D67">
         <v>124</v>
       </c>
-      <c r="E67" t="s">
-        <v>48</v>
+      <c r="E67" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -1260,13 +1304,13 @@
         <v>1</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D70">
         <v>125</v>
       </c>
-      <c r="E70" t="s">
-        <v>48</v>
+      <c r="E70" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -1287,13 +1331,13 @@
         <v>1</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D73">
         <v>125</v>
       </c>
-      <c r="E73" t="s">
-        <v>49</v>
+      <c r="E73" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="74" spans="1:6">
@@ -1309,13 +1353,13 @@
         <v>1</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D75">
         <v>127</v>
       </c>
-      <c r="E75" t="s">
-        <v>49</v>
+      <c r="E75" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="76" spans="1:6">
@@ -1326,16 +1370,16 @@
         <v>1</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D76">
         <v>127</v>
       </c>
-      <c r="E76" t="s">
-        <v>48</v>
-      </c>
-      <c r="F76" t="s">
-        <v>54</v>
+      <c r="E76" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="77" spans="1:6">
@@ -1351,13 +1395,13 @@
         <v>1</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D78">
         <v>124</v>
       </c>
-      <c r="E78" t="s">
-        <v>48</v>
+      <c r="E78" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="79" spans="1:6">
@@ -1370,7 +1414,7 @@
         <v>1979</v>
       </c>
     </row>
-    <row r="81" spans="1:5">
+    <row r="81" spans="1:6">
       <c r="A81">
         <v>1980</v>
       </c>
@@ -1378,26 +1422,26 @@
         <v>1</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D81">
         <v>125</v>
       </c>
-      <c r="E81" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5">
+      <c r="E81" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6">
       <c r="A82">
         <v>1981</v>
       </c>
     </row>
-    <row r="83" spans="1:5">
+    <row r="83" spans="1:6">
       <c r="A83">
         <v>1982</v>
       </c>
     </row>
-    <row r="84" spans="1:5">
+    <row r="84" spans="1:6">
       <c r="A84">
         <v>1983</v>
       </c>
@@ -1405,16 +1449,16 @@
         <v>1</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D84">
         <v>125</v>
       </c>
-      <c r="E84" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5">
+      <c r="E84" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6">
       <c r="A85">
         <v>1984</v>
       </c>
@@ -1422,26 +1466,26 @@
         <v>1</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D85">
         <v>148</v>
       </c>
-      <c r="E85" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5">
+      <c r="E85" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6">
       <c r="A86">
         <v>1985</v>
       </c>
     </row>
-    <row r="87" spans="1:5">
+    <row r="87" spans="1:6">
       <c r="A87">
         <v>1986</v>
       </c>
     </row>
-    <row r="88" spans="1:5">
+    <row r="88" spans="1:6">
       <c r="A88">
         <v>1987</v>
       </c>
@@ -1449,26 +1493,29 @@
         <v>1</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D88">
         <v>148</v>
       </c>
-      <c r="E88" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5">
+      <c r="E88" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F88" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6">
       <c r="A89">
         <v>1988</v>
       </c>
     </row>
-    <row r="90" spans="1:5">
+    <row r="90" spans="1:6">
       <c r="A90">
         <v>1989</v>
       </c>
     </row>
-    <row r="91" spans="1:5">
+    <row r="91" spans="1:6">
       <c r="A91">
         <v>1990</v>
       </c>
@@ -1476,26 +1523,26 @@
         <v>1</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D91">
         <v>148</v>
       </c>
-      <c r="E91" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5">
+      <c r="E91" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6">
       <c r="A92">
         <v>1991</v>
       </c>
     </row>
-    <row r="93" spans="1:5">
+    <row r="93" spans="1:6">
       <c r="A93">
         <v>1992</v>
       </c>
     </row>
-    <row r="94" spans="1:5">
+    <row r="94" spans="1:6">
       <c r="A94">
         <v>1993</v>
       </c>
@@ -1503,21 +1550,21 @@
         <v>1</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D94">
         <v>147</v>
       </c>
-      <c r="E94" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5">
+      <c r="E94" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6">
       <c r="A95">
         <v>1994</v>
       </c>
     </row>
-    <row r="96" spans="1:5">
+    <row r="96" spans="1:6">
       <c r="A96">
         <v>1995</v>
       </c>
@@ -1530,16 +1577,16 @@
         <v>1</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D97">
         <v>148</v>
       </c>
-      <c r="E97" t="s">
-        <v>48</v>
-      </c>
-      <c r="F97" t="s">
-        <v>55</v>
+      <c r="E97" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F97" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="98" spans="1:6">
@@ -1555,13 +1602,13 @@
         <v>1</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D99">
         <v>148</v>
       </c>
-      <c r="E99" t="s">
-        <v>48</v>
+      <c r="E99" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="100" spans="1:6">
@@ -1582,13 +1629,13 @@
         <v>1</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D102">
         <v>150</v>
       </c>
-      <c r="E102" t="s">
-        <v>48</v>
+      <c r="E102" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="103" spans="1:6">
@@ -1609,13 +1656,13 @@
         <v>1</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D105">
         <v>150</v>
       </c>
-      <c r="E105" t="s">
-        <v>48</v>
+      <c r="E105" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="106" spans="1:6">
@@ -1636,16 +1683,16 @@
         <v>1</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D108">
         <v>150</v>
       </c>
-      <c r="E108" t="s">
-        <v>49</v>
-      </c>
-      <c r="F108" t="s">
-        <v>56</v>
+      <c r="E108" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F108" s="1" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="109" spans="1:6">
@@ -1666,13 +1713,13 @@
         <v>1</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D111">
         <v>150</v>
       </c>
-      <c r="E111" t="s">
-        <v>49</v>
+      <c r="E111" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="112" spans="1:6">
@@ -1693,13 +1740,13 @@
         <v>1</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D114">
         <v>150</v>
       </c>
-      <c r="E114" t="s">
-        <v>48</v>
+      <c r="E114" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="115" spans="1:5">
@@ -1720,13 +1767,13 @@
         <v>1</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D117">
         <v>150</v>
       </c>
-      <c r="E117" t="s">
-        <v>48</v>
+      <c r="E117" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="118" spans="1:5">

</xml_diff>